<commit_message>
added nosocomial and fungal infection panels
</commit_message>
<xml_diff>
--- a/inst/taxidpanels/Panels.xlsx
+++ b/inst/taxidpanels/Panels.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selkamand/projects/r_packages/microbialpanels/inst/taxidpanels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4310AD-1398-0C44-AE26-77668193FBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497EFEC6-0EF1-D147-8E80-BFD0B5B2B3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37280" yWindow="-6900" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DE75A970-BC08-AF41-8450-250134611CA6}"/>
+    <workbookView xWindow="12200" yWindow="1460" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DE75A970-BC08-AF41-8450-250134611CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="HumanMicrobiomeLarge" sheetId="1" r:id="rId1"/>
     <sheet name="OralMicrobiome" sheetId="5" r:id="rId2"/>
     <sheet name="CancerViruses" sheetId="2" r:id="rId3"/>
-    <sheet name="TorqueTenoVirusesSpecies" sheetId="3" r:id="rId4"/>
-    <sheet name="TorqueTenoVirusesGenus" sheetId="4" r:id="rId5"/>
+    <sheet name="CommonNosocomial" sheetId="6" r:id="rId4"/>
+    <sheet name="FungalPathogens" sheetId="7" r:id="rId5"/>
+    <sheet name="TorqueTenoVirusesSpecies" sheetId="3" r:id="rId6"/>
+    <sheet name="TorqueTenoVirusesGenus" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="182">
   <si>
     <t>Taxid</t>
   </si>
@@ -496,6 +498,159 @@
   </si>
   <si>
     <t>https://doi.org/10.1186/s12985-018-1007-6</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Fungi</t>
+  </si>
+  <si>
+    <t>Candida albicans</t>
+  </si>
+  <si>
+    <t>Crptococcus</t>
+  </si>
+  <si>
+    <t>Aspergillus</t>
+  </si>
+  <si>
+    <r>
+      <t>Candida</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tropicalis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Candida</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parapsilosis</t>
+    </r>
+  </si>
+  <si>
+    <t>Pichia kudriavzevii</t>
+  </si>
+  <si>
+    <t>Clavispora lusitaniae</t>
+  </si>
+  <si>
+    <t>Cryptococcosis</t>
+  </si>
+  <si>
+    <t>Aspergillosis</t>
+  </si>
+  <si>
+    <t>Mucorales</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1093/jpids/pix046 </t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix047</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix048</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix049</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix050</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix051</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix052</t>
+  </si>
+  <si>
+    <t>10.1093/jpids/pix053</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Proteus mirabilis</t>
+  </si>
+  <si>
+    <t>Clostridioides difficile</t>
+  </si>
+  <si>
+    <t>Enterococcus sp.</t>
+  </si>
+  <si>
+    <t>Streptococcus viridans</t>
+  </si>
+  <si>
+    <t>Citrobacter freundii</t>
+  </si>
+  <si>
+    <r>
+      <t>Enterobacter</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sp.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -604,10 +759,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,8 +777,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3580,7 +3738,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F1" activeCellId="5" sqref="A1 D1 C1 E1 G1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3910,10 +4068,373 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50DEBF7-68E0-E448-872A-F18BC891D2CD}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1280</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>573</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>287</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>42895</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7">
+        <v>562</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>546</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>584</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>78535</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>35783</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1496</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi?mode=Tree&amp;id=1496&amp;lvl=3&amp;keep=1&amp;srchmode=1&amp;unlock" xr:uid="{93A0A4FD-257B-634D-A5CA-5020B8C55B16}"/>
+    <hyperlink ref="A7" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi?mode=Tree&amp;id=546&amp;lvl=3&amp;keep=1&amp;srchmode=1&amp;unlock" xr:uid="{EA6B8331-3EA2-6D4B-A892-7910ED93F50D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEB75CF-C77F-074A-8674-B970362D146D}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2">
+        <v>5052</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5476</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>5482</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5">
+        <v>5480</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6">
+        <v>4909</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7">
+        <v>36911</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8">
+        <v>5206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9">
+        <v>4827</v>
+      </c>
+      <c r="D9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0C8B71-BC4C-7C44-AB72-C976B5CF8D25}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -4417,7 +4938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C84DE7F-90DF-904F-913D-FA6A628B1542}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: added Primate T-lymphotropic virus 2 due to expected similarity with virus 1
</commit_message>
<xml_diff>
--- a/inst/taxidpanels/Panels.xlsx
+++ b/inst/taxidpanels/Panels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selkamand/projects/r_packages/microbialpanels/inst/taxidpanels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497EFEC6-0EF1-D147-8E80-BFD0B5B2B3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D818A236-F54E-D548-9D6F-1766D54A4A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="1460" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DE75A970-BC08-AF41-8450-250134611CA6}"/>
+    <workbookView xWindow="8200" yWindow="1460" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{DE75A970-BC08-AF41-8450-250134611CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="HumanMicrobiomeLarge" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="186">
   <si>
     <t>Taxid</t>
   </si>
@@ -652,12 +652,24 @@
       <t xml:space="preserve"> sp.</t>
     </r>
   </si>
+  <si>
+    <t>Primate T-lymphotropic virus 2</t>
+  </si>
+  <si>
+    <t>HTLV1</t>
+  </si>
+  <si>
+    <t>HTLV2</t>
+  </si>
+  <si>
+    <t>Only putatively identified as associated with cancer. Included due to expected simliarity to HTLV1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -741,6 +753,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -768,16 +791,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -797,9 +820,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -837,7 +860,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -943,7 +966,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1085,7 +1108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1102,7 +1125,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1127,7 +1149,7 @@
       <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1153,7 +1175,7 @@
       <c r="G2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1179,7 +1201,7 @@
       <c r="G3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1205,7 +1227,7 @@
       <c r="G4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1231,7 +1253,7 @@
       <c r="G5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1257,7 +1279,7 @@
       <c r="G6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1283,7 +1305,7 @@
       <c r="G7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1309,7 +1331,7 @@
       <c r="G8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1335,7 +1357,7 @@
       <c r="G9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1361,7 +1383,7 @@
       <c r="G10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1387,7 +1409,7 @@
       <c r="G11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1413,7 +1435,7 @@
       <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1439,7 +1461,7 @@
       <c r="G13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1465,7 +1487,7 @@
       <c r="G14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1491,7 +1513,7 @@
       <c r="G15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1517,7 +1539,7 @@
       <c r="G16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1543,7 +1565,7 @@
       <c r="G17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1569,7 +1591,7 @@
       <c r="G18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1595,7 +1617,7 @@
       <c r="G19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1621,7 +1643,7 @@
       <c r="G20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1647,7 +1669,7 @@
       <c r="G21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1673,7 +1695,7 @@
       <c r="G22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1699,7 +1721,7 @@
       <c r="G23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1725,7 +1747,7 @@
       <c r="G24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1751,7 +1773,7 @@
       <c r="G25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1777,7 +1799,7 @@
       <c r="G26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1803,7 +1825,7 @@
       <c r="G27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1829,7 +1851,7 @@
       <c r="G28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1855,7 +1877,7 @@
       <c r="G29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1881,7 +1903,7 @@
       <c r="G30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1907,7 +1929,7 @@
       <c r="G31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1933,7 +1955,7 @@
       <c r="G32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1959,7 +1981,7 @@
       <c r="G33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1985,7 +2007,7 @@
       <c r="G34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2011,7 +2033,7 @@
       <c r="G35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2037,7 +2059,7 @@
       <c r="G36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2063,7 +2085,7 @@
       <c r="G37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2089,7 +2111,7 @@
       <c r="G38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2115,7 +2137,7 @@
       <c r="G39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2141,7 +2163,7 @@
       <c r="G40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2167,7 +2189,7 @@
       <c r="G41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2193,7 +2215,7 @@
       <c r="G42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2219,7 +2241,7 @@
       <c r="G43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H43" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2245,7 +2267,7 @@
       <c r="G44" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2271,7 +2293,7 @@
       <c r="G45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2297,7 +2319,7 @@
       <c r="G46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2323,7 +2345,7 @@
       <c r="G47" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2349,7 +2371,7 @@
       <c r="G48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2375,7 +2397,7 @@
       <c r="G49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2401,7 +2423,7 @@
       <c r="G50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="H50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2427,7 +2449,7 @@
       <c r="G51" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2453,7 +2475,7 @@
       <c r="G52" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2479,7 +2501,7 @@
       <c r="G53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2505,7 +2527,7 @@
       <c r="G54" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2531,7 +2553,7 @@
       <c r="G55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2557,7 +2579,7 @@
       <c r="G56" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2583,7 +2605,7 @@
       <c r="G57" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2609,7 +2631,7 @@
       <c r="G58" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2635,7 +2657,7 @@
       <c r="G59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2661,7 +2683,7 @@
       <c r="G60" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2687,7 +2709,7 @@
       <c r="G61" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2713,7 +2735,7 @@
       <c r="G62" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2739,7 +2761,7 @@
       <c r="G63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2765,7 +2787,7 @@
       <c r="G64" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2791,7 +2813,7 @@
       <c r="G65" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2817,7 +2839,7 @@
       <c r="G66" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2843,7 +2865,7 @@
       <c r="G67" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2869,7 +2891,7 @@
       <c r="G68" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2895,7 +2917,7 @@
       <c r="G69" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2921,7 +2943,7 @@
       <c r="G70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2947,7 +2969,7 @@
       <c r="G71" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2973,7 +2995,7 @@
       <c r="G72" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2999,7 +3021,7 @@
       <c r="G73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3025,7 +3047,7 @@
       <c r="G74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3051,7 +3073,7 @@
       <c r="G75" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H75" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3077,7 +3099,7 @@
       <c r="G76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3103,7 +3125,7 @@
       <c r="G77" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3129,7 +3151,7 @@
       <c r="G78" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3155,7 +3177,7 @@
       <c r="G79" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3181,7 +3203,7 @@
       <c r="G80" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H80" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3207,7 +3229,7 @@
       <c r="G81" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3484,247 +3506,247 @@
       <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>28037</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>39777</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>1379</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>1304</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="C5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>43675</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>28132</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="C7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>484</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="C8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>1318</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>34026</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>137732</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3735,10 +3757,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9628375D-A715-A445-B59F-C4C599BBC0F6}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" activeCellId="5" sqref="A1 D1 C1 E1 G1 F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3746,6 +3768,7 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3772,293 +3795,334 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="11">
         <v>37296</v>
       </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>10376</v>
       </c>
-      <c r="E3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>32603</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="11">
         <v>32604</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>10372</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>146</v>
       </c>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="11">
         <v>194440</v>
       </c>
-      <c r="E7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="13">
+        <v>194441</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="11">
         <v>10566</v>
       </c>
-      <c r="E8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="11">
         <v>10407</v>
       </c>
-      <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="11">
         <v>11103</v>
       </c>
-      <c r="E10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="E11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="11">
         <v>493803</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D12">
+      <c r="D13" s="11">
         <v>1891767</v>
       </c>
-      <c r="E12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="E13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="11">
         <v>1891763</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="E14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="11">
         <v>1891762</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="E15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="11">
         <v>10358</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="11">
         <v>687331</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F17" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G17" s="11" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4071,7 +4135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50DEBF7-68E0-E448-872A-F18BC891D2CD}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -4135,7 +4199,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>287</v>
       </c>
       <c r="D4" t="s">
@@ -4163,7 +4227,7 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>562</v>
       </c>
       <c r="D6" t="s">
@@ -4171,7 +4235,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>180</v>
       </c>
       <c r="B7" t="s">
@@ -4227,7 +4291,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>177</v>
       </c>
       <c r="B11" t="s">
@@ -4444,21 +4508,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B2" t="s">
@@ -4472,7 +4536,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
@@ -4486,7 +4550,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B4" t="s">
@@ -4500,7 +4564,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B5" t="s">
@@ -4514,7 +4578,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="18">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B6" t="s">
@@ -4528,7 +4592,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="18">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B7" t="s">
@@ -4542,7 +4606,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="18">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B8" t="s">
@@ -4556,7 +4620,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="18">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B9" t="s">
@@ -4570,7 +4634,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="18">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B10" t="s">
@@ -4584,7 +4648,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="18">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B11" t="s">
@@ -4598,7 +4662,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="18">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B12" t="s">
@@ -4612,7 +4676,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="18">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B13" t="s">
@@ -4626,7 +4690,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="18">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B14" t="s">
@@ -4640,7 +4704,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="18">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B15" t="s">
@@ -4654,7 +4718,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="18">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B16" t="s">
@@ -4668,7 +4732,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="18">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B17" t="s">
@@ -4682,7 +4746,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B18" t="s">
@@ -4696,7 +4760,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="18">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B19" t="s">
@@ -4710,7 +4774,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="18">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B20" t="s">
@@ -4724,7 +4788,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B21" t="s">
@@ -4738,7 +4802,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="18">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B22" t="s">
@@ -4752,7 +4816,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="18">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B23" t="s">
@@ -4766,7 +4830,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="18">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B24" t="s">
@@ -4780,7 +4844,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="18">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B25" t="s">
@@ -4794,7 +4858,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="18">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B26" t="s">
@@ -4808,7 +4872,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="18">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>121</v>
       </c>
       <c r="B27" t="s">
@@ -4822,7 +4886,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="18">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B28" t="s">
@@ -4836,7 +4900,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B29" t="s">
@@ -4850,7 +4914,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="18">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B30" t="s">
@@ -4864,7 +4928,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B31" t="s">
@@ -4878,7 +4942,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="18">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B32" t="s">
@@ -4892,7 +4956,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="18">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B33" t="s">
@@ -4906,7 +4970,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="18">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B34" t="s">
@@ -4920,7 +4984,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="18">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B35" t="s">
@@ -4952,16 +5016,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>